<commit_message>
update supp table 2 path, rerun
</commit_message>
<xml_diff>
--- a/tables/results/SuppTable2-Molecular-Subtype-Table.xlsx
+++ b/tables/results/SuppTable2-Molecular-Subtype-Table.xlsx
@@ -5326,14 +5326,16 @@
         <v>290</v>
       </c>
       <c r="E40" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F40"/>
       <c r="G40"/>
       <c r="H40" t="s">
         <v>163</v>
       </c>
-      <c r="I40"/>
+      <c r="I40" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
@@ -5457,14 +5459,16 @@
         <v>290</v>
       </c>
       <c r="E45" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45" t="s">
         <v>163</v>
       </c>
-      <c r="I45"/>
+      <c r="I45" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
@@ -5567,14 +5571,16 @@
         <v>313</v>
       </c>
       <c r="E49" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F49"/>
       <c r="G49"/>
       <c r="H49" t="s">
         <v>163</v>
       </c>
-      <c r="I49"/>
+      <c r="I49" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
@@ -5590,14 +5596,16 @@
         <v>290</v>
       </c>
       <c r="E50" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F50"/>
       <c r="G50"/>
       <c r="H50" t="s">
         <v>163</v>
       </c>
-      <c r="I50"/>
+      <c r="I50" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
@@ -5856,14 +5864,16 @@
         <v>290</v>
       </c>
       <c r="E60" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F60"/>
       <c r="G60"/>
       <c r="H60" t="s">
         <v>163</v>
       </c>
-      <c r="I60"/>
+      <c r="I60" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
@@ -5933,14 +5943,16 @@
         <v>290</v>
       </c>
       <c r="E63" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F63"/>
       <c r="G63"/>
       <c r="H63" t="s">
         <v>163</v>
       </c>
-      <c r="I63"/>
+      <c r="I63" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
@@ -6093,14 +6105,16 @@
         <v>290</v>
       </c>
       <c r="E69" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F69"/>
       <c r="G69"/>
       <c r="H69" t="s">
         <v>163</v>
       </c>
-      <c r="I69"/>
+      <c r="I69" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
@@ -6425,14 +6439,16 @@
         <v>290</v>
       </c>
       <c r="E81" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F81"/>
       <c r="G81"/>
       <c r="H81" t="s">
         <v>163</v>
       </c>
-      <c r="I81"/>
+      <c r="I81" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
@@ -6477,14 +6493,16 @@
         <v>290</v>
       </c>
       <c r="E83" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F83"/>
       <c r="G83"/>
       <c r="H83" t="s">
         <v>163</v>
       </c>
-      <c r="I83"/>
+      <c r="I83" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
@@ -7005,14 +7023,16 @@
         <v>290</v>
       </c>
       <c r="E103" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F103"/>
       <c r="G103"/>
       <c r="H103" t="s">
         <v>163</v>
       </c>
-      <c r="I103"/>
+      <c r="I103" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
@@ -8437,14 +8457,16 @@
         <v>290</v>
       </c>
       <c r="E157" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F157"/>
       <c r="G157"/>
       <c r="H157" t="s">
         <v>163</v>
       </c>
-      <c r="I157"/>
+      <c r="I157" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
@@ -8819,14 +8841,16 @@
         <v>290</v>
       </c>
       <c r="E171" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F171"/>
       <c r="G171"/>
       <c r="H171" t="s">
         <v>163</v>
       </c>
-      <c r="I171"/>
+      <c r="I171" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
@@ -9301,14 +9325,16 @@
         <v>290</v>
       </c>
       <c r="E189" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F189"/>
       <c r="G189"/>
       <c r="H189" t="s">
         <v>163</v>
       </c>
-      <c r="I189"/>
+      <c r="I189" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
@@ -9974,14 +10000,16 @@
         <v>313</v>
       </c>
       <c r="E214" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F214"/>
       <c r="G214"/>
       <c r="H214" t="s">
         <v>163</v>
       </c>
-      <c r="I214"/>
+      <c r="I214" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="s">
@@ -10346,14 +10374,16 @@
         <v>290</v>
       </c>
       <c r="E228" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F228"/>
       <c r="G228"/>
       <c r="H228" t="s">
         <v>163</v>
       </c>
-      <c r="I228"/>
+      <c r="I228" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
@@ -10784,14 +10814,16 @@
         <v>290</v>
       </c>
       <c r="E244" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="F244"/>
       <c r="G244"/>
       <c r="H244" t="s">
         <v>163</v>
       </c>
-      <c r="I244"/>
+      <c r="I244" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="s">

</xml_diff>